<commit_message>
Finish up facings and modify exclusions
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/MSC/Data/MSC Template v1.1.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/MSC/Data/MSC Template v1.1.xlsx
@@ -5,14 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Availability" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Double Availability" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Presence" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Facings" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Facings" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="89">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -101,9 +100,6 @@
     <t xml:space="preserve">In-Store Activation Q5 KO minicans</t>
   </si>
   <si>
-    <t xml:space="preserve">Presence</t>
-  </si>
-  <si>
     <t xml:space="preserve">In-Store Activation Q6 Tie in rate of Coke Zero Sugar</t>
   </si>
   <si>
@@ -167,13 +163,25 @@
     <t xml:space="preserve">att3</t>
   </si>
   <si>
+    <t xml:space="preserve">att4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minimum facings</t>
   </si>
   <si>
-    <t xml:space="preserve">Store Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXCLUDE</t>
+    <t xml:space="preserve">Minimum Brands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excluded_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excluded_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_of_sub_packages</t>
   </si>
   <si>
     <t xml:space="preserve">CCNA</t>
@@ -185,7 +193,10 @@
     <t xml:space="preserve">SSD MULTI-SERVE,TRANSACTION PACKAGE,SSD IC</t>
   </si>
   <si>
-    <t xml:space="preserve">12OZ CANS (att 1)</t>
+    <t xml:space="preserve">additional_attribute_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12OZ CANS</t>
   </si>
   <si>
     <t xml:space="preserve">GOLD PEAK TEA,HONEST TEA,PEACE TEA</t>
@@ -197,6 +208,9 @@
     <t xml:space="preserve">DASANI WATER,DASANI SPARKLING,SMARTWATER,SMARTWATER SPARKLING,TOPO CHICO</t>
   </si>
   <si>
+    <t xml:space="preserve">*Hunter has asked for possible name replacements for 'att1' and 'att3'. Ask Uri or whoever what would be the best name to give the attributes found in these fields</t>
+  </si>
+  <si>
     <t xml:space="preserve">FANTA ORANGE,FANTA PINEAPPLE</t>
   </si>
   <si>
@@ -209,16 +223,28 @@
     <t xml:space="preserve">DUNKIN DONUTS,MC CAFE,</t>
   </si>
   <si>
-    <t xml:space="preserve">On-Prem</t>
-  </si>
-  <si>
     <t xml:space="preserve">*How do I indicate a lead brand *No unique call for Monster JAVA</t>
   </si>
   <si>
     <t xml:space="preserve">GOLD PEAK TEA,HONEST TEA,PEACE TEA,FUZE</t>
   </si>
   <si>
-    <t xml:space="preserve">*Hunter has asked for possible name replacements for 'att1' and 'att3'. Ask Uri or whoever what would be the best name to give the attributes found in these fields</t>
+    <t xml:space="preserve">COKE CLASSIC,COKE DT,COKE CHERRY,COKE ZERO,COKE ZERO CF,COKE CHERRY ZERO,COKE ZERO SUGAR,FANTA,SPRITE,SPRITE ZERO,SEAGRAMS,FRESCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6,10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COKE CLASSIC,COKE ZERO SUGAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BARQS ROOT BEER,COKE CLASSIC,COKE DT,COKE ZERO SUGAR,SPRITE,MELLO YELLO,SEAGRAMS,FRESCA,FANTA ORANGE,PIBB XTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DASANI WATER,DASANI SPARKLING,SMARTWATER,SMARTWATER SPARKLING</t>
   </si>
   <si>
     <t xml:space="preserve">Brand Group 1</t>
@@ -239,39 +265,6 @@
     <t xml:space="preserve">MONSTER COFFEE+ENERGY</t>
   </si>
   <si>
-    <t xml:space="preserve">size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number_of_sub_packages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Brands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">att4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COKE CLASSIC,COKE DT,COKE CHERRY,COKE ZERO,COKE ZERO CF,COKE CHERRY ZERO,COKE ZERO SUGAR,FANTA,SPRITE,SPRITE ZERO,SEAGRAMS,FRESCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COKE CLASSIC,COKE ZERO SUGAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BARQS ROOT BEER,COKE CLASSIC,COKE DT,COKE ZERO SUGAR,SPRITE,MELLO YELLO,SEAGRAMS,FRESCA,FANTA ORANGE,PIBB XTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DASANI WATER,DASANI SPARKLING,SMARTWATER,SMARTWATER SPARKLING</t>
-  </si>
-  <si>
     <t xml:space="preserve">numerator_types</t>
   </si>
   <si>
@@ -284,7 +277,7 @@
     <t xml:space="preserve">denominator_value</t>
   </si>
   <si>
-    <t xml:space="preserve">EXCLUDED</t>
+    <t xml:space="preserve">brand_name</t>
   </si>
   <si>
     <t xml:space="preserve">BARQS ROOT BEER,FANTA BERRY,COKE VANILLA,PIBB XTRA,COKE CLASSIC,COKE DT,Coke Diet Lime,Coke Diet with Splenda,PIBB ZERO,POWERADE,POWERADE ZERO,Mello Yello Cherry,FANTA APPLE,FANTA GRAPEFRUIT,FANTA CHERRY,SEAGRAMS,COKE VANILLA ZERO,SMARTWATER,SPRITE,Honest Kids,SPRITE CRANBERRY,Odwalla,SPRITE ZERO,SURGE,COKE CHERRY,TAB,GLACEAU VITAMIN WATER,CORE POWER,GLACEAU VITAMIN WATER ZERO,Delaware Punch,Fanta Fruit Punch,COKE CF DT,ZICO COCONUT WATER,COKE ZERO,COKE ZERO CF,DASANI DROPS,DASANI SPARKLING,DASANI WATER,COKE LIFE,FANTA GRAPE,FANTA MANGO,Aloe Gloe,GOLD PEAK TEA,FANTA ORANGE,FANTA ORANGE ZERO,HONEST TEA,FANTA PINEAPPLE,FUZE,FANTA STRAWBERRY,FRESCA,FRUITWATER,COKE CLASSIC CF,COKE CHERRY ZERO,COKE CHERRY DT,MELLO YELLO,SMARTWATER SPARKLING,PEACE TEA,GOLD PEAK COFFEE,DUNKIN DONUTS,ILLY FREDDO,MELLO YELLO ZERO,SPRITE CRANBERRY ZERO,YUP,Hi-C,Tum-E Yummies,FANTA PEACH,COKE ZERO SUGAR,HONEST,HONEST FIZZ,SPRITE CHERRY,SPRITE CHERRY ZERO,HONEST Juice,FANTA GREEN APPLE,MC CAFE,TOPO CHICO,RED FLASH,FAIRLIFE,ALOE REY</t>
@@ -525,14 +518,14 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="63.0111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.8888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="63.0111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="64.5777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.6518518518518"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="64.5777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +682,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -697,10 +690,10 @@
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -708,10 +701,10 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -719,43 +712,43 @@
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>17</v>
@@ -763,10 +756,10 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -774,53 +767,53 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -839,204 +832,315 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.1777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.8037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="57.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.5444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.237037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.8814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6925925925926"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="58.7962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" s="8" customFormat="true" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="8" t="n">
+        <v>65</v>
+      </c>
+      <c r="G7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="0" t="s">
-        <v>64</v>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1063,12 +1167,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,19 +1180,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,10 +1200,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>6</v>
@@ -1108,7 +1212,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1116,10 +1220,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>6</v>
@@ -1128,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2"/>
     </row>
@@ -1148,289 +1252,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="131.507407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.41111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.41111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.1444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>